<commit_message>
Column for max. contracted length
added a column for maximum contracted PAM length, theoretical (25%) and measured.
</commit_message>
<xml_diff>
--- a/Knee Torque Test Jig/Testing Data/10mmFesto_Mar2021/RawData_Mar2021.xlsx
+++ b/Knee Torque Test Jig/Testing Data/10mmFesto_Mar2021/RawData_Mar2021.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Research\Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben Bolen\Documents\GitHub\Bipedal_Robot\Knee Torque Test Jig\Testing Data\10mmFesto_Mar2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8827B821-8CDD-4D82-B6B0-AF13D89F650E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47329950-780B-4450-84E7-345FE570EC21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C5028A70-FE19-46E9-AE6B-5AA55AFE7839}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" firstSheet="4" activeTab="6" xr2:uid="{C5028A70-FE19-46E9-AE6B-5AA55AFE7839}"/>
   </bookViews>
   <sheets>
     <sheet name="Calibration" sheetId="1" r:id="rId1"/>
@@ -194,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="45">
   <si>
     <t>Zero Factor(Horizontal Configuration)</t>
   </si>
@@ -321,6 +321,15 @@
   <si>
     <t>**NOTE:  Extension Data is first series of data collected.  Throughout Extension tests and even into Flexsion tests, number of data points collected per knee angle was increased from 150 pts to 6000 pts</t>
   </si>
+  <si>
+    <t>theoretical</t>
+  </si>
+  <si>
+    <t>measured</t>
+  </si>
+  <si>
+    <t>Max contracted length</t>
+  </si>
 </sst>
 </file>
 
@@ -397,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -431,13 +440,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,10 +465,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -758,7 +766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8180AF-8C44-45A9-AFCE-AB9E07AFCB68}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -1429,7 +1437,7 @@
       <c r="C42">
         <v>31.450700000000001</v>
       </c>
-      <c r="F42" s="17">
+      <c r="F42" s="15">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
@@ -1642,7 +1650,7 @@
       <c r="C57">
         <v>43.536499999999997</v>
       </c>
-      <c r="F57" s="17">
+      <c r="F57" s="15">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
@@ -2590,7 +2598,7 @@
       <c r="F5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="16" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2604,7 +2612,7 @@
       <c r="F6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="15"/>
+      <c r="G6" s="16"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -3122,7 +3130,7 @@
       <c r="H5" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="16" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3139,7 +3147,7 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="12"/>
-      <c r="I6" s="15"/>
+      <c r="I6" s="16"/>
     </row>
     <row r="7" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
@@ -3154,7 +3162,7 @@
       <c r="H7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="15"/>
+      <c r="I7" s="16"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
@@ -5104,19 +5112,20 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{015E007F-60E8-4779-AD66-7B1F859103FD}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="63.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>20</v>
       </c>
@@ -5129,8 +5138,11 @@
       <c r="D1" s="10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F1" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -5144,8 +5156,14 @@
         <f>C2</f>
         <v>23.8125</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -5159,8 +5177,12 @@
         <f>C3</f>
         <v>385.76249999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F3">
+        <f>C3*0.75</f>
+        <v>289.32187499999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -5170,12 +5192,12 @@
       <c r="C4" s="8">
         <v>63.5</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="17">
         <f>SUM(C4:C6)</f>
         <v>168.27500000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -5185,9 +5207,9 @@
       <c r="C5" s="8">
         <v>23.8125</v>
       </c>
-      <c r="D5" s="16"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D5" s="17"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -5197,9 +5219,9 @@
       <c r="C6" s="8">
         <v>80.962500000000006</v>
       </c>
-      <c r="D6" s="16"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D6" s="17"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>16</v>
       </c>
@@ -5210,8 +5232,11 @@
         <v>14</v>
       </c>
       <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F8" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -5221,8 +5246,14 @@
       <c r="C9" s="2">
         <v>25.4</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -5232,8 +5263,12 @@
       <c r="C10" s="2">
         <v>361.95</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F10">
+        <f>C10*0.75</f>
+        <v>271.46249999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -5244,7 +5279,7 @@
         <v>142.875</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>21</v>
       </c>

</xml_diff>